<commit_message>
Added formulas and charts exercises.
</commit_message>
<xml_diff>
--- a/formulas/income-by-quarters.xlsx
+++ b/formulas/income-by-quarters.xlsx
@@ -10,6 +10,11 @@
     <sheet name="Exercise" sheetId="1" r:id="rId1"/>
     <sheet name="Solution" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="FIXED_COMISSION">Exercise!$B$14</definedName>
+    <definedName name="TAXES">Exercise!$B$16</definedName>
+    <definedName name="VARIABLE_COMMISION">Exercise!$B$15</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -20,12 +25,6 @@
     <t>INCOME</t>
   </si>
   <si>
-    <t>FIXED COMMISIONS</t>
-  </si>
-  <si>
-    <t>VARIABLE COMMISIONS</t>
-  </si>
-  <si>
     <t>EBT</t>
   </si>
   <si>
@@ -63,6 +62,12 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>FIXED COMMISSIONS</t>
+  </si>
+  <si>
+    <t>VARIABLE COMMISSIONS</t>
   </si>
 </sst>
 </file>
@@ -71,7 +76,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;€&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -198,12 +203,6 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -242,18 +241,18 @@
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -266,6 +265,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +283,220 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="120"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="20"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Annual Income Partitioning</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Solution!$A$5,Solution!$A$6,Solution!$A$9,Solution!$A$11)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FIXED COMMISSIONS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VARIABLE COMMISSIONS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TAXES</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PAT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Solution!$F$5:$F$6,Solution!$F$9,Solution!$F$11)</c:f>
+              <c:numCache>
+                <c:formatCode>"€"#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>416000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>414400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>769600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent5"/>
+    </a:solidFill>
+    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent5">
+          <a:shade val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,7 +789,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,186 +802,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15">
+        <v>480000</v>
+      </c>
+      <c r="C4" s="15">
+        <v>560000</v>
+      </c>
+      <c r="D4" s="15">
+        <v>320000</v>
+      </c>
+      <c r="E4" s="15">
+        <v>720000</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="17">
-        <v>480000</v>
-      </c>
-      <c r="C4" s="17">
-        <v>560000</v>
-      </c>
-      <c r="D4" s="17">
-        <v>320000</v>
-      </c>
-      <c r="E4" s="17">
-        <v>720000</v>
-      </c>
-      <c r="F4" s="24"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="B14" s="13">
+        <v>120000</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="15">
-        <v>120000</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="16">
+      <c r="B16" s="14">
         <v>0.35</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -792,264 +1011,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>480000</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <v>560000</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>320000</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="15">
         <v>720000</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="16">
         <f>SUM(B4:E4)</f>
         <v>2080000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="15">
+        <f>FIXED_COMISSION</f>
+        <v>120000</v>
+      </c>
+      <c r="C5" s="15">
+        <f>FIXED_COMISSION</f>
+        <v>120000</v>
+      </c>
+      <c r="D5" s="15">
+        <f>FIXED_COMISSION</f>
+        <v>120000</v>
+      </c>
+      <c r="E5" s="15">
+        <f>FIXED_COMISSION</f>
+        <v>120000</v>
+      </c>
+      <c r="F5" s="15">
+        <f>FIXED_COMISSION</f>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="15">
+        <f>B4*VARIABLE_COMMISION</f>
+        <v>96000</v>
+      </c>
+      <c r="C6" s="15">
+        <f>C4*VARIABLE_COMMISION</f>
+        <v>112000</v>
+      </c>
+      <c r="D6" s="15">
+        <f>D4*VARIABLE_COMMISION</f>
+        <v>64000</v>
+      </c>
+      <c r="E6" s="15">
+        <f>E4*VARIABLE_COMMISION</f>
+        <v>144000</v>
+      </c>
+      <c r="F6" s="15">
+        <f>F4*VARIABLE_COMMISION</f>
+        <v>416000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17">
-        <f>$B14</f>
-        <v>120000</v>
-      </c>
-      <c r="C5" s="17">
-        <f t="shared" ref="C5:E5" si="0">$B14</f>
-        <v>120000</v>
-      </c>
-      <c r="D5" s="17">
-        <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
-      <c r="E5" s="17">
-        <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
-      <c r="F5" s="18">
-        <f t="shared" ref="F5:F11" si="1">SUM(B5:E5)</f>
-        <v>480000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17">
-        <f>B4*$B15</f>
-        <v>96000</v>
-      </c>
-      <c r="C6" s="17">
-        <f t="shared" ref="C6:E6" si="2">C4*$B15</f>
-        <v>112000</v>
-      </c>
-      <c r="D6" s="17">
-        <f t="shared" si="2"/>
-        <v>64000</v>
-      </c>
-      <c r="E6" s="17">
-        <f t="shared" si="2"/>
-        <v>144000</v>
-      </c>
-      <c r="F6" s="17">
-        <f t="shared" si="1"/>
-        <v>416000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <f>B4-B5-B6</f>
         <v>264000</v>
       </c>
-      <c r="C7" s="19">
-        <f t="shared" ref="C7:E7" si="3">C4-C5-C6</f>
+      <c r="C7" s="17">
+        <f t="shared" ref="C7:E7" si="0">C4-C5-C6</f>
         <v>328000</v>
       </c>
-      <c r="D7" s="19">
-        <f t="shared" si="3"/>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
         <v>136000</v>
       </c>
-      <c r="E7" s="19">
-        <f t="shared" si="3"/>
+      <c r="E7" s="17">
+        <f t="shared" si="0"/>
         <v>456000</v>
       </c>
-      <c r="F7" s="20">
-        <f t="shared" si="1"/>
+      <c r="F7" s="18">
+        <f t="shared" ref="F7:F11" si="1">SUM(B7:E7)</f>
         <v>1184000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="17">
-        <f>B7*$B16</f>
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15">
+        <f>B7*TAXES</f>
         <v>92400</v>
       </c>
-      <c r="C9" s="17">
-        <f t="shared" ref="C9:E9" si="4">C7*$B16</f>
+      <c r="C9" s="15">
+        <f>C7*TAXES</f>
         <v>114799.99999999999</v>
       </c>
-      <c r="D9" s="17">
-        <f t="shared" si="4"/>
+      <c r="D9" s="15">
+        <f>D7*TAXES</f>
         <v>47600</v>
       </c>
-      <c r="E9" s="17">
-        <f t="shared" si="4"/>
+      <c r="E9" s="15">
+        <f>E7*TAXES</f>
         <v>159600</v>
       </c>
-      <c r="F9" s="18">
-        <f t="shared" si="1"/>
+      <c r="F9" s="15">
+        <f>F7*TAXES</f>
         <v>414400</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="21">
+      <c r="A11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="19">
         <f>B7-B9</f>
         <v>171600</v>
       </c>
-      <c r="C11" s="21">
-        <f t="shared" ref="C11:E11" si="5">C7-C9</f>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:E11" si="2">C7-C9</f>
         <v>213200</v>
       </c>
-      <c r="D11" s="21">
-        <f t="shared" si="5"/>
+      <c r="D11" s="19">
+        <f t="shared" si="2"/>
         <v>88400</v>
       </c>
-      <c r="E11" s="21">
-        <f t="shared" si="5"/>
+      <c r="E11" s="19">
+        <f t="shared" si="2"/>
         <v>296400</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="20">
         <f t="shared" si="1"/>
         <v>769600</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="13">
+        <v>120000</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15">
-        <v>120000</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <v>0.2</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="4"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="16">
+      <c r="A16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="14">
         <v>0.35</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1057,5 +1276,6 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>